<commit_message>
Beginning of Data Scaping
</commit_message>
<xml_diff>
--- a/JAR-StockManager/Data/StockData.xlsx
+++ b/JAR-StockManager/Data/StockData.xlsx
@@ -1,111 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <x:workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature_Workspace\Jar-P2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5928bd39eca494ab/Documents/UiPath/Jar-P2/JAR-StockManager/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BD9841-BC78-4924-B254-715E4832D124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="735" yWindow="1440" windowWidth="27420" windowHeight="13800" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="162913"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{07BD9841-BC78-4924-B254-715E4832D124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D97CAEB9-A0C8-4505-8FFD-EA35762CC3FD}"/>
+  <bookViews>
+    <workbookView xWindow="3576" yWindow="1320" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <x:si>
-    <x:t>Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AMZN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AAPL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NASDAQ</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>NASDAQ</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,47 +354,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D1"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C4" sqref="C4 C4:C4"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="17.285156" style="1" customWidth="1"/>
-    <x:col min="2" max="2" width="15.285156" style="1" customWidth="1"/>
-    <x:col min="3" max="3" width="15.710938" style="1" customWidth="1"/>
-    <x:col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <x:col min="5" max="5" width="15.285156" style="1" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="C4" s="1" t="s"/>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
one iteration of adding data to excel
</commit_message>
<xml_diff>
--- a/JAR-StockManager/Data/StockData.xlsx
+++ b/JAR-StockManager/Data/StockData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5928bd39eca494ab/Documents/UiPath/Jar-P2/JAR-StockManager/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{07BD9841-BC78-4924-B254-715E4832D124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D97CAEB9-A0C8-4505-8FFD-EA35762CC3FD}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{07BD9841-BC78-4924-B254-715E4832D124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA531D78-4559-4F5A-9508-0B6151FF2401}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="1320" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="1404" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
   <si>
     <t>AMZN</t>
   </si>
   <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>NASDAQ</t>
-  </si>
-  <si>
-    <t>Time</t>
+    <t>WEN</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>123.75</t>
+  </si>
+  <si>
+    <t>3,158.00</t>
+  </si>
+  <si>
+    <t>22.02</t>
+  </si>
+  <si>
+    <t>641.76</t>
+  </si>
+  <si>
+    <t>214.29</t>
   </si>
 </sst>
 </file>
@@ -355,31 +376,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10 C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>